<commit_message>
ultimando detalles de excel 3,4,6
</commit_message>
<xml_diff>
--- a/src/test/resources/Descriptions/DC_AUT_001_Biometricos.xlsx
+++ b/src/test/resources/Descriptions/DC_AUT_001_Biometricos.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20394"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20FDE2CB-4AB3-40C8-BD56-333FEA17DFB0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34369F10-B954-41CE-9AD7-F6F6021D60A4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -484,7 +484,7 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="45.42578125" customWidth="1"/>
-    <col min="2" max="2" width="31.140625" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" customWidth="1"/>
     <col min="3" max="3" width="47.28515625" customWidth="1"/>
     <col min="4" max="4" width="40.7109375" customWidth="1"/>
     <col min="5" max="5" width="41" customWidth="1"/>

</xml_diff>